<commit_message>
Documented some rows to explain parameters
</commit_message>
<xml_diff>
--- a/generic cluster v2.xlsx
+++ b/generic cluster v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SGlazerman\Documents\Mathematica Backup 2019\Documents\Professional and Staff Development\Power analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SGlazerman\Documents\0. Peru Trip\Power analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F73E06B-6A92-4284-B5FE-994ED818C713}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D2DDC6-731E-4695-8A1C-8BDF1FA0480A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generic Cluster RA" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
   <si>
     <t>2-tailed, 10% significance, 80% power ==&gt; constant = 2.48</t>
   </si>
@@ -142,14 +142,32 @@
   <si>
     <t>Note: Still need to make these changes to the other tabs (RA at level 2 and binary outcome)</t>
   </si>
+  <si>
+    <t>&lt;-- uses t distribution with DF correction</t>
+  </si>
+  <si>
+    <t>&lt;-- Should almost always be "2"</t>
+  </si>
+  <si>
+    <t>&lt;-- Should almost always be 0.05</t>
+  </si>
+  <si>
+    <t>&lt;-- Should almost always be 0.80</t>
+  </si>
+  <si>
+    <t>&lt;-- Make this specific to the study context</t>
+  </si>
+  <si>
+    <t>&lt;-- Your best estimate based on your study design</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -249,13 +267,13 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -263,8 +281,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -581,10 +599,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -592,17 +612,17 @@
     <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -622,7 +642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
@@ -641,8 +661,11 @@
       <c r="F5" s="8">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
@@ -661,8 +684,11 @@
       <c r="F6" s="9">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
@@ -681,8 +707,11 @@
       <c r="F7" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -695,7 +724,7 @@
         <v>2.8056568516240223</v>
       </c>
       <c r="D8" s="7">
-        <f t="shared" ref="C8:F8" si="0">_xlfn.T.INV(D5,D17-D15-D11)+_xlfn.T.INV((1-(D6/D7)),D17-D15-D11)</f>
+        <f t="shared" ref="D8:F8" si="0">_xlfn.T.INV(D5,D17-D15-D11)+_xlfn.T.INV((1-(D6/D7)),D17-D15-D11)</f>
         <v>2.8046343001142713</v>
       </c>
       <c r="E8" s="7">
@@ -706,8 +735,11 @@
         <f t="shared" si="0"/>
         <v>2.80259849723222</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -726,8 +758,11 @@
       <c r="F9" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -746,8 +781,11 @@
       <c r="F10" s="8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>26</v>
       </c>
@@ -766,8 +804,11 @@
       <c r="F11" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -786,8 +827,11 @@
       <c r="F12" s="8">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>27</v>
       </c>
@@ -806,8 +850,11 @@
       <c r="F13" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -827,7 +874,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -933,7 +980,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1164,7 +1211,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>